<commit_message>
standard deviation + start charts
</commit_message>
<xml_diff>
--- a/template/report_template.xlsx
+++ b/template/report_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\עבודה פרילנסרית\Etzion\Etzion Code Projects\EAPC-light-train-red-line\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86C5600F-8712-40EA-BA6D-D4BAC8FC2C2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C12CFF00-8D0B-4524-AF2C-0F3E01F33D40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="9780" windowHeight="10170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="41">
   <si>
     <t xml:space="preserve">דוח מעקב  - יחידת ניטור MetriCorr ICL </t>
   </si>
@@ -67,9 +67,6 @@
   </si>
   <si>
     <t xml:space="preserve"> DC Current density</t>
-  </si>
-  <si>
-    <t xml:space="preserve">פוטנציאל EIR </t>
   </si>
   <si>
     <t>VAC</t>
@@ -134,15 +131,9 @@
     <t>ממוצע</t>
   </si>
   <si>
-    <t>[דקות]</t>
-  </si>
-  <si>
     <t>מתחת ל-0 וולט</t>
   </si>
   <si>
-    <t>מעל ל-1.5- וולט</t>
-  </si>
-  <si>
     <t>מעל ל-0.03 A/m²</t>
   </si>
   <si>
@@ -150,13 +141,31 @@
   </si>
   <si>
     <t>מעל ל-850- מיליוולט</t>
+  </si>
+  <si>
+    <t xml:space="preserve">פוטנציאל Eon </t>
+  </si>
+  <si>
+    <t>מעל ל-1.15- וולט</t>
+  </si>
+  <si>
+    <t>[שניות]</t>
+  </si>
+  <si>
+    <t>סטיית תקן</t>
+  </si>
+  <si>
+    <t>XXX</t>
+  </si>
+  <si>
+    <t>*שעון UTC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -187,6 +196,20 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -208,7 +231,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -218,9 +241,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -249,7 +271,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>184150</xdr:colOff>
+      <xdr:colOff>215900</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>69295</xdr:rowOff>
     </xdr:to>
@@ -556,21 +578,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A8:J43"/>
+  <dimension ref="A8:J48"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView rightToLeft="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="21.6328125" customWidth="1"/>
-    <col min="2" max="2" width="12.54296875" customWidth="1"/>
+    <col min="2" max="2" width="16.26953125" customWidth="1"/>
     <col min="3" max="3" width="4.81640625" customWidth="1"/>
-    <col min="4" max="4" width="11.26953125" customWidth="1"/>
-    <col min="5" max="5" width="17.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.7265625" customWidth="1"/>
+    <col min="5" max="5" width="16.90625" customWidth="1"/>
     <col min="6" max="6" width="5.81640625" customWidth="1"/>
-    <col min="7" max="7" width="11.26953125" customWidth="1"/>
+    <col min="7" max="7" width="7.6328125" customWidth="1"/>
     <col min="8" max="8" width="19" customWidth="1"/>
     <col min="9" max="9" width="6.6328125" customWidth="1"/>
     <col min="10" max="10" width="7.26953125" customWidth="1"/>
@@ -594,6 +616,10 @@
       <c r="C10" t="s">
         <v>2</v>
       </c>
+      <c r="D10" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="6"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
@@ -609,28 +635,31 @@
         <v>5</v>
       </c>
       <c r="B14" s="4"/>
+      <c r="C14" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C16" s="3">
-        <v>500</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>28</v>
+        <v>1</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="E16" t="s">
         <v>7</v>
       </c>
       <c r="F16" s="3">
-        <v>499</v>
+        <v>1</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
@@ -643,8 +672,8 @@
       <c r="C17" s="3">
         <v>1</v>
       </c>
-      <c r="D17" s="5" t="s">
-        <v>28</v>
+      <c r="D17" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
@@ -662,212 +691,208 @@
         <v>10</v>
       </c>
       <c r="C19">
-        <v>-1.1000000000000001</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>29</v>
+        <v>1</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="E19" t="s">
         <v>11</v>
       </c>
       <c r="F19">
-        <v>-1</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>29</v>
+        <v>1</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" s="2"/>
       <c r="B20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E20" t="s">
+        <v>38</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A21" s="2"/>
+      <c r="B21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21">
+        <v>4.33</v>
+      </c>
+      <c r="D21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="D22" s="3"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A23" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E23" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A24" s="2"/>
+      <c r="B24" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E24" t="s">
+        <v>38</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A25" s="2"/>
+      <c r="B25" t="s">
+        <v>36</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="D26" s="3"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A27" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E27" t="s">
+        <v>11</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A28" s="4"/>
+      <c r="B28" t="s">
         <v>31</v>
       </c>
-      <c r="C20">
-        <v>-1.1000000000000001</v>
-      </c>
-      <c r="D20" s="5" t="s">
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="D29" s="3"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A30" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" t="s">
+        <v>10</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E20" t="s">
-        <v>34</v>
-      </c>
-      <c r="F20">
-        <v>4.33</v>
-      </c>
-      <c r="G20" t="s">
+      <c r="E30" t="s">
+        <v>11</v>
+      </c>
+      <c r="F30">
+        <v>1</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A31" s="4"/>
+      <c r="B31" t="s">
+        <v>30</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E31" t="s">
+        <v>38</v>
+      </c>
+      <c r="F31">
+        <v>1</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A32" s="4"/>
+      <c r="B32" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="D21" s="3"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A22" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B22" t="s">
-        <v>10</v>
-      </c>
-      <c r="C22">
-        <v>-1.1000000000000001</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E22" t="s">
-        <v>11</v>
-      </c>
-      <c r="F22">
-        <v>-1</v>
-      </c>
-      <c r="G22" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A23" s="2"/>
-      <c r="B23" t="s">
-        <v>31</v>
-      </c>
-      <c r="C23">
-        <v>5</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E23" t="s">
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32" t="s">
         <v>37</v>
-      </c>
-      <c r="F23">
-        <v>4.33</v>
-      </c>
-      <c r="G23" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="D24" s="3"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A25" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B25" t="s">
-        <v>10</v>
-      </c>
-      <c r="C25">
-        <v>0.8</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E25" t="s">
-        <v>11</v>
-      </c>
-      <c r="F25">
-        <v>-0.3</v>
-      </c>
-      <c r="G25" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A26" s="4"/>
-      <c r="B26" t="s">
-        <v>33</v>
-      </c>
-      <c r="C26">
-        <v>4.33</v>
-      </c>
-      <c r="D26" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="D27" s="3"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A28" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B28" t="s">
-        <v>10</v>
-      </c>
-      <c r="C28">
-        <v>-1.1000000000000001</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E28" t="s">
-        <v>11</v>
-      </c>
-      <c r="G28" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A29" s="4"/>
-      <c r="B29" t="s">
-        <v>31</v>
-      </c>
-      <c r="C29">
-        <v>-1.1000000000000001</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E29" t="s">
-        <v>35</v>
-      </c>
-      <c r="F29">
-        <v>4.33</v>
-      </c>
-      <c r="G29" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="D30" s="3"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A31" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B31" t="s">
-        <v>10</v>
-      </c>
-      <c r="C31">
-        <v>-1.1000000000000001</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E31" t="s">
-        <v>11</v>
-      </c>
-      <c r="G31" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B32" t="s">
-        <v>31</v>
-      </c>
-      <c r="C32">
-        <v>-1.1000000000000001</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E32" t="s">
-        <v>16</v>
-      </c>
-      <c r="F32">
-        <v>4.33</v>
-      </c>
-      <c r="G32" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.35">
@@ -875,94 +900,162 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B34" t="s">
         <v>10</v>
       </c>
       <c r="C34">
-        <v>-1.1000000000000001</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>30</v>
+        <v>1</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="E34" t="s">
         <v>11</v>
       </c>
-      <c r="G34" s="5" t="s">
-        <v>30</v>
+      <c r="F34">
+        <v>1</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B35" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C35">
-        <v>-1.1000000000000001</v>
-      </c>
-      <c r="D35" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E35" t="s">
+        <v>38</v>
+      </c>
+      <c r="F35">
+        <v>1</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B36" t="s">
+        <v>15</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+      <c r="D36" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D37" s="3"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A38" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B38" t="s">
+        <v>10</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E38" t="s">
+        <v>11</v>
+      </c>
+      <c r="F38">
+        <v>1</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B39" t="s">
         <v>30</v>
       </c>
-      <c r="E35" t="s">
-        <v>36</v>
-      </c>
-      <c r="F35">
-        <v>4.33</v>
-      </c>
-      <c r="G35" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="D36" s="5"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A38" s="1" t="s">
+      <c r="C39">
+        <v>1</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E39" t="s">
+        <v>38</v>
+      </c>
+      <c r="F39">
+        <v>1</v>
+      </c>
+      <c r="G39" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B40" t="s">
+        <v>33</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
+      </c>
+      <c r="D40" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A43" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
+      <c r="B45" t="s">
         <v>20</v>
       </c>
-      <c r="B40" t="s">
+      <c r="C45" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
         <v>21</v>
       </c>
-      <c r="C40" t="s">
+      <c r="B46" t="s">
+        <v>20</v>
+      </c>
+      <c r="C46" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>22</v>
+      </c>
+      <c r="B47" t="s">
+        <v>20</v>
+      </c>
+      <c r="C47" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
-        <v>22</v>
-      </c>
-      <c r="B41" t="s">
-        <v>21</v>
-      </c>
-      <c r="C41" t="s">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
-        <v>23</v>
-      </c>
-      <c r="B42" t="s">
-        <v>21</v>
-      </c>
-      <c r="C42" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
-        <v>27</v>
-      </c>
-      <c r="B43" t="s">
-        <v>21</v>
-      </c>
-      <c r="C43" t="s">
-        <v>25</v>
+      <c r="B48" t="s">
+        <v>20</v>
+      </c>
+      <c r="C48" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>